<commit_message>
tab def trans grales
</commit_message>
<xml_diff>
--- a/6- Ingenieria de producto/6.1 - Análisis/04- Archivos de Trabajo/MID - Tablas Definidas.xlsx
+++ b/6- Ingenieria de producto/6.1 - Análisis/04- Archivos de Trabajo/MID - Tablas Definidas.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Tablas Def Entidad" sheetId="1" r:id="rId1"/>
-    <sheet name="Tablas Transacciones Entidad" sheetId="2" r:id="rId2"/>
-    <sheet name="Tablas Transacciones Grales" sheetId="3" r:id="rId3"/>
+    <sheet name="Tablas TransaccionesGenerales " sheetId="4" r:id="rId2"/>
+    <sheet name="Old" sheetId="2" r:id="rId3"/>
+    <sheet name="Old 1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -73,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K19" authorId="0">
+    <comment ref="K18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0">
+    <comment ref="K19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G30" authorId="0">
+    <comment ref="G22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="163">
   <si>
     <t>Tipo Entidad</t>
   </si>
@@ -566,13 +567,55 @@
   </si>
   <si>
     <t>Impuesto a las Ganancias</t>
+  </si>
+  <si>
+    <t>TipoTransacción</t>
+  </si>
+  <si>
+    <t>Base Descuento</t>
+  </si>
+  <si>
+    <t>Sueldo Básico</t>
+  </si>
+  <si>
+    <t>Sueldo Bruto</t>
+  </si>
+  <si>
+    <t>Ayuda económica</t>
+  </si>
+  <si>
+    <t>ImpactoDescuento</t>
+  </si>
+  <si>
+    <t>Embargo</t>
+  </si>
+  <si>
+    <t>Beneficio</t>
+  </si>
+  <si>
+    <t>Cuota alimentaria</t>
+  </si>
+  <si>
+    <t>Beneficiario</t>
+  </si>
+  <si>
+    <t>Impuesto</t>
+  </si>
+  <si>
+    <t>ParteAplicación</t>
+  </si>
+  <si>
+    <t>Parcial</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,6 +704,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -708,7 +758,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -762,6 +812,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,7 +1122,7 @@
   <dimension ref="B2:V54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1627,11 +1681,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="34" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O38"/>
+  <dimension ref="C2:O31"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1706,16 +1852,24 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="G11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>23</v>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.3">
@@ -1723,10 +1877,10 @@
         <v>25</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="K12" s="7">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.3">
@@ -1734,10 +1888,7 @@
         <v>28</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" s="7">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.3">
@@ -1745,12 +1896,15 @@
         <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="G15" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="G17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.3">
@@ -1758,11 +1912,11 @@
         <v>35</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="G18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>37</v>
+      <c r="G18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="8">
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.3">
@@ -1770,22 +1924,16 @@
         <v>38</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K19" s="8">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="8">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
@@ -1796,107 +1944,97 @@
       <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="K26" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C27" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="K27" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="G28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="G29" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C30" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="G30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>24</v>
+      <c r="G30" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="G32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="K34" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="K35" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J36" s="9"/>
-    </row>
-    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G37" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G38" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1906,12 +2044,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>